<commit_message>
Prepared Scrum Board (Second Sprint First Cycle)
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint1/Sprint Backlog.xlsx
+++ b/Project/Phase 2/Sprint1/Sprint Backlog.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\IdeaProjects\OliveiraGant\ganttproject\Project\Phase 2\Sprint1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2302F203-6AA6-4368-AD28-936B8CD7A933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,25 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Reviewing</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +52,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +381,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Decided on tasks for second cycle
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint1/Sprint Backlog.xlsx
+++ b/Project/Phase 2/Sprint1/Sprint Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\IdeaProjects\OliveiraGant\ganttproject\Project\Phase 2\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2302F203-6AA6-4368-AD28-936B8CD7A933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B666428-32D5-4740-BE1B-021F70BB1AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Todo</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Sugerir 2 Features (Francisco)</t>
+  </si>
+  <si>
+    <t>Sugerir 2 Features (Iago)</t>
+  </si>
+  <si>
+    <t>Sugerir 2 Features (James)</t>
+  </si>
+  <si>
+    <t>Sugerir 2 Features (Joao)</t>
+  </si>
+  <si>
+    <t>Sugerir 2 Features (Ricardo)</t>
   </si>
 </sst>
 </file>
@@ -382,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,6 +425,31 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>